<commit_message>
Use new class MasterSolutionList to get ids and validate solutions
Now read ID<->solutions list from a CSV file. This is use to validate
solutions and find the IDs associated with them. Also now accents are
stripped from puzzle-specific code where needed. The canonicalize
utility method strips accents (it has a hardcoded list of accents for
the moment).
Bricks and Clocks have been update to this new scheme.
</commit_message>
<xml_diff>
--- a/GAU2017/administrative/puzzle-phrases.xlsx
+++ b/GAU2017/administrative/puzzle-phrases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
   <si>
     <t>Jupiter</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>IN</t>
   </si>
 </sst>
 </file>
@@ -691,485 +694,608 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="42.21875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="42.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f xml:space="preserve"> ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f t="shared" ref="A3:A31" si="0" xml:space="preserve"> ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>73</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>74</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>64</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>65</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>77</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>94</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>66</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>78</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>96</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>67</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>79</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>98</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>81</v>
-      </c>
-      <c r="C11">
-        <v>10080</v>
       </c>
       <c r="D11">
         <v>10080</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>10080</v>
+      </c>
+      <c r="F11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>82</v>
-      </c>
-      <c r="C12">
-        <v>3600</v>
       </c>
       <c r="D12">
         <v>3600</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>3600</v>
+      </c>
+      <c r="F12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>83</v>
-      </c>
-      <c r="C13">
-        <v>1440</v>
       </c>
       <c r="D13">
         <v>1440</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>1440</v>
+      </c>
+      <c r="F13" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>84</v>
-      </c>
-      <c r="C14">
-        <v>36</v>
       </c>
       <c r="D14">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>85</v>
-      </c>
-      <c r="C15">
-        <v>48</v>
       </c>
       <c r="D15">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>86</v>
-      </c>
-      <c r="C16">
-        <v>60</v>
       </c>
       <c r="D16">
         <v>60</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>87</v>
-      </c>
-      <c r="C17">
-        <v>72</v>
       </c>
       <c r="D17">
         <v>72</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>72</v>
+      </c>
+      <c r="F17" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>88</v>
-      </c>
-      <c r="C18">
-        <v>84</v>
       </c>
       <c r="D18">
         <v>84</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>84</v>
+      </c>
+      <c r="F18" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>89</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>90</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>91</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>92</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>93</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>70</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>71</v>
-      </c>
-      <c r="C24">
-        <v>1000</v>
       </c>
       <c r="D24">
         <v>1000</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>1000</v>
+      </c>
+      <c r="F24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>23</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>39</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>40</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>41</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>21</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>43</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>22</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Got CountCells integrated, added animal name to solution phrases
- Added the 10 countCell solutions to puzzle-phrases.txt
- Added a bunch of animal names to puzzle-phrases.txt - for lasers.
- CountCells code integrated
- Added CountCells parameterized puzzle generator
genOverlappingRectsPuzzle
- Changed solution-table.csv name to puzzle-phrases.csv to match the
excel name.
</commit_message>
<xml_diff>
--- a/GAU2017/administrative/puzzle-phrases.xlsx
+++ b/GAU2017/administrative/puzzle-phrases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="147">
   <si>
     <t>Jupiter</t>
   </si>
@@ -326,13 +326,145 @@
     <t>agua</t>
   </si>
   <si>
-    <t>IsNumber</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>IN</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>for CC</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Búfalo</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>Camello</t>
+  </si>
+  <si>
+    <t>Deer</t>
+  </si>
+  <si>
+    <t>Venado</t>
+  </si>
+  <si>
+    <t>Elephant</t>
+  </si>
+  <si>
+    <t>Elefante</t>
+  </si>
+  <si>
+    <t>Giraffe</t>
+  </si>
+  <si>
+    <t>Jirafa</t>
+  </si>
+  <si>
+    <t>Gorilla</t>
+  </si>
+  <si>
+    <t>Gorila</t>
+  </si>
+  <si>
+    <t>Horse</t>
+  </si>
+  <si>
+    <t>Caballo</t>
+  </si>
+  <si>
+    <t>Kangaroo</t>
+  </si>
+  <si>
+    <t>Canguro</t>
+  </si>
+  <si>
+    <t>Leopard</t>
+  </si>
+  <si>
+    <t>Leopardo</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
+  </si>
+  <si>
+    <t>Conejo</t>
+  </si>
+  <si>
+    <t>Squirrel</t>
+  </si>
+  <si>
+    <t>Ardilla</t>
+  </si>
+  <si>
+    <t>Whale</t>
+  </si>
+  <si>
+    <t>Bellena</t>
+  </si>
+  <si>
+    <t>Dolphin</t>
+  </si>
+  <si>
+    <t>Delfín</t>
+  </si>
+  <si>
+    <t>Crow</t>
+  </si>
+  <si>
+    <t>Cuervo</t>
+  </si>
+  <si>
+    <t>Dove</t>
+  </si>
+  <si>
+    <t>Paloma</t>
+  </si>
+  <si>
+    <t>Eagle</t>
+  </si>
+  <si>
+    <t>Águila</t>
+  </si>
+  <si>
+    <t>Flamingo</t>
+  </si>
+  <si>
+    <t>Flamenco</t>
+  </si>
+  <si>
+    <t>Hummingbird</t>
+  </si>
+  <si>
+    <t>Colibrí</t>
+  </si>
+  <si>
+    <t>Ostrich</t>
+  </si>
+  <si>
+    <t>Avestruz</t>
+  </si>
+  <si>
+    <t>Parrot</t>
+  </si>
+  <si>
+    <t>Papagayo</t>
+  </si>
+  <si>
+    <t>Pelican</t>
+  </si>
+  <si>
+    <t>Pelicano</t>
+  </si>
+  <si>
+    <t>Pigeon</t>
+  </si>
+  <si>
+    <t>Quetzal</t>
   </si>
 </sst>
 </file>
@@ -694,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,7 +840,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -723,7 +855,7 @@
         <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -746,7 +878,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f t="shared" ref="A3:A31" si="0" xml:space="preserve"> ROW()-1</f>
+        <f t="shared" ref="A3:A64" si="0" xml:space="preserve"> ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -905,9 +1037,6 @@
       <c r="E11">
         <v>10080</v>
       </c>
-      <c r="F11" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -926,9 +1055,6 @@
       <c r="E12">
         <v>3600</v>
       </c>
-      <c r="F12" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -947,9 +1073,6 @@
       <c r="E13">
         <v>1440</v>
       </c>
-      <c r="F13" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -968,9 +1091,6 @@
       <c r="E14">
         <v>36</v>
       </c>
-      <c r="F14" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -989,9 +1109,6 @@
       <c r="E15">
         <v>48</v>
       </c>
-      <c r="F15" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1010,9 +1127,6 @@
       <c r="E16">
         <v>60</v>
       </c>
-      <c r="F16" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1031,9 +1145,6 @@
       <c r="E17">
         <v>72</v>
       </c>
-      <c r="F17" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -1052,9 +1163,6 @@
       <c r="E18">
         <v>84</v>
       </c>
-      <c r="F18" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
@@ -1109,9 +1217,6 @@
       <c r="E21">
         <v>4</v>
       </c>
-      <c r="F21" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1130,9 +1235,6 @@
       <c r="E22">
         <v>2</v>
       </c>
-      <c r="F22" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -1169,9 +1271,6 @@
       <c r="E24">
         <v>1000</v>
       </c>
-      <c r="F24" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -1297,6 +1396,630 @@
       </c>
       <c r="E31" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>69</v>
+      </c>
+      <c r="C32">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>69</v>
+      </c>
+      <c r="E32">
+        <v>69</v>
+      </c>
+      <c r="F32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>68</v>
+      </c>
+      <c r="C33">
+        <v>68</v>
+      </c>
+      <c r="D33">
+        <v>68</v>
+      </c>
+      <c r="E33">
+        <v>68</v>
+      </c>
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>64</v>
+      </c>
+      <c r="C34">
+        <v>64</v>
+      </c>
+      <c r="D34">
+        <v>64</v>
+      </c>
+      <c r="E34">
+        <v>64</v>
+      </c>
+      <c r="F34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>62</v>
+      </c>
+      <c r="C35">
+        <v>62</v>
+      </c>
+      <c r="D35">
+        <v>62</v>
+      </c>
+      <c r="E35">
+        <v>62</v>
+      </c>
+      <c r="F35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>66</v>
+      </c>
+      <c r="C36">
+        <v>66</v>
+      </c>
+      <c r="D36">
+        <v>66</v>
+      </c>
+      <c r="E36">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>60</v>
+      </c>
+      <c r="D37">
+        <v>60</v>
+      </c>
+      <c r="E37">
+        <v>60</v>
+      </c>
+      <c r="F37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>55</v>
+      </c>
+      <c r="C38">
+        <v>55</v>
+      </c>
+      <c r="D38">
+        <v>55</v>
+      </c>
+      <c r="E38">
+        <v>55</v>
+      </c>
+      <c r="F38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>53</v>
+      </c>
+      <c r="C39">
+        <v>53</v>
+      </c>
+      <c r="D39">
+        <v>53</v>
+      </c>
+      <c r="E39">
+        <v>53</v>
+      </c>
+      <c r="F39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>46</v>
+      </c>
+      <c r="D40">
+        <v>46</v>
+      </c>
+      <c r="E40">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>54</v>
+      </c>
+      <c r="C41">
+        <v>54</v>
+      </c>
+      <c r="D41">
+        <v>54</v>
+      </c>
+      <c r="E41">
+        <v>54</v>
+      </c>
+      <c r="F41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" t="s">
+        <v>111</v>
+      </c>
+      <c r="E46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" t="s">
+        <v>115</v>
+      </c>
+      <c r="E48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51" t="s">
+        <v>121</v>
+      </c>
+      <c r="E51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
+        <v>126</v>
+      </c>
+      <c r="D53" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="s">
+        <v>128</v>
+      </c>
+      <c r="D54" t="s">
+        <v>127</v>
+      </c>
+      <c r="E54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" t="s">
+        <v>129</v>
+      </c>
+      <c r="E55" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56" t="s">
+        <v>131</v>
+      </c>
+      <c r="E56" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" t="s">
+        <v>133</v>
+      </c>
+      <c r="E57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" t="s">
+        <v>135</v>
+      </c>
+      <c r="E58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" t="s">
+        <v>139</v>
+      </c>
+      <c r="E60" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>141</v>
+      </c>
+      <c r="C61" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>143</v>
+      </c>
+      <c r="C62" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" t="s">
+        <v>143</v>
+      </c>
+      <c r="E62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" t="s">
+        <v>146</v>
+      </c>
+      <c r="E64" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>